<commit_message>
[FIX] Inventory 버그 수정
</commit_message>
<xml_diff>
--- a/Assets/Resources/ItemData/ItemExcel.xlsx
+++ b/Assets/Resources/ItemData/ItemExcel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity\Team\EscapeIsekai\Assets\ExcelFile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity\Team\EscapeIsekai\Assets\Resources\ItemData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA165CD-FF3B-4128-8E89-35CE403D709A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007C6617-9F32-4508-997B-B85869D6BC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{23FCFA80-21D9-4745-B9DA-57060EA57FF8}"/>
+    <workbookView xWindow="2580" yWindow="2655" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{23FCFA80-21D9-4745-B9DA-57060EA57FF8}"/>
   </bookViews>
   <sheets>
     <sheet name="ItemDatas" sheetId="1" r:id="rId1"/>
@@ -38,16 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
-  <si>
-    <t>_id</t>
-  </si>
-  <si>
-    <t>_itemName</t>
-  </si>
-  <si>
-    <t>_itemExplanation</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
   <si>
     <t>나무 검</t>
   </si>
@@ -94,16 +85,6 @@
     <t>퀘스트 아이템</t>
   </si>
   <si>
-    <t>_price</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>_dropPrefabPath</t>
-  </si>
-  <si>
-    <t>_iconPath</t>
-  </si>
-  <si>
     <t>Prefabs/Entities/DropItem/0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -120,53 +101,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>_maxCount</t>
-  </si>
-  <si>
-    <t>_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>_hp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>_temperature</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>_atk</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>_def</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>_speed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>_stamina</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>_isStat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>_craftingPrice</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>_craftingID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>_isCrafting</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>나무 검의 레시피</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -207,18 +141,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>_availableCount</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>_materials_string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>_materials_count_string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Sprite/Icon/2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -240,6 +162,86 @@
   </si>
   <si>
     <t>Sprite/Icon/7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>itemName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>itemExplanation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dropPrefabPath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iconPath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>maxCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isStat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isCrafting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>temperature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>atk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>def</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>speed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stamina</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>craftingID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>craftingPrice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>materials_string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>materials_count_string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>availableCount</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -606,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36525DF8-9879-4440-9A1B-CB7EE677C95C}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -623,31 +625,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="G1" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="H1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="I1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -655,19 +657,19 @@
         <v>10010000</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -684,19 +686,19 @@
         <v>10200000</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -713,19 +715,19 @@
         <v>10001000</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -742,19 +744,19 @@
         <v>10002000</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D5">
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -771,19 +773,19 @@
         <v>10000000</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D6">
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -800,19 +802,19 @@
         <v>10100000</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
         <v>15</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
       <c r="F7" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="G7">
         <v>99</v>
@@ -829,19 +831,19 @@
         <v>10300000</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D8">
         <v>100</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="G8">
         <v>99</v>
@@ -858,19 +860,19 @@
         <v>10400000</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -887,19 +889,19 @@
         <v>10110000</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="G10">
         <v>99</v>
@@ -916,19 +918,19 @@
         <v>10110001</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="G11">
         <v>99</v>
@@ -945,19 +947,19 @@
         <v>10110002</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F12" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="G12">
         <v>99</v>
@@ -974,19 +976,19 @@
         <v>10110003</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F13" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="G13">
         <v>99</v>
@@ -1003,19 +1005,19 @@
         <v>10110004</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F14" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="G14">
         <v>99</v>
@@ -1038,7 +1040,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1049,25 +1051,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="F1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="G1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1218,8 +1220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAB882E2-DC2B-4364-A1E7-50F2FE65D6AC}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1234,22 +1236,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Kdh fix inventory (#54)
* [FIX] Inventory 버그 수정

* [FIX] 초기화 순서 조정 및 private 필드명 수정

* [UPDATE] 누락코드 수정
</commit_message>
<xml_diff>
--- a/Assets/Resources/ItemData/ItemExcel.xlsx
+++ b/Assets/Resources/ItemData/ItemExcel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity\Team\EscapeIsekai\Assets\ExcelFile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity\Team\EscapeIsekai\Assets\Resources\ItemData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA165CD-FF3B-4128-8E89-35CE403D709A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007C6617-9F32-4508-997B-B85869D6BC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{23FCFA80-21D9-4745-B9DA-57060EA57FF8}"/>
+    <workbookView xWindow="2580" yWindow="2655" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{23FCFA80-21D9-4745-B9DA-57060EA57FF8}"/>
   </bookViews>
   <sheets>
     <sheet name="ItemDatas" sheetId="1" r:id="rId1"/>
@@ -38,16 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
-  <si>
-    <t>_id</t>
-  </si>
-  <si>
-    <t>_itemName</t>
-  </si>
-  <si>
-    <t>_itemExplanation</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
   <si>
     <t>나무 검</t>
   </si>
@@ -94,16 +85,6 @@
     <t>퀘스트 아이템</t>
   </si>
   <si>
-    <t>_price</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>_dropPrefabPath</t>
-  </si>
-  <si>
-    <t>_iconPath</t>
-  </si>
-  <si>
     <t>Prefabs/Entities/DropItem/0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -120,53 +101,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>_maxCount</t>
-  </si>
-  <si>
-    <t>_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>_hp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>_temperature</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>_atk</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>_def</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>_speed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>_stamina</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>_isStat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>_craftingPrice</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>_craftingID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>_isCrafting</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>나무 검의 레시피</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -207,18 +141,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>_availableCount</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>_materials_string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>_materials_count_string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Sprite/Icon/2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -240,6 +162,86 @@
   </si>
   <si>
     <t>Sprite/Icon/7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>itemName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>itemExplanation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dropPrefabPath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iconPath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>maxCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isStat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isCrafting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>temperature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>atk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>def</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>speed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stamina</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>craftingID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>craftingPrice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>materials_string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>materials_count_string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>availableCount</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -606,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36525DF8-9879-4440-9A1B-CB7EE677C95C}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -623,31 +625,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="G1" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="H1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="I1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -655,19 +657,19 @@
         <v>10010000</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -684,19 +686,19 @@
         <v>10200000</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -713,19 +715,19 @@
         <v>10001000</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -742,19 +744,19 @@
         <v>10002000</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D5">
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -771,19 +773,19 @@
         <v>10000000</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D6">
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -800,19 +802,19 @@
         <v>10100000</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
         <v>15</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
       <c r="F7" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="G7">
         <v>99</v>
@@ -829,19 +831,19 @@
         <v>10300000</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D8">
         <v>100</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="G8">
         <v>99</v>
@@ -858,19 +860,19 @@
         <v>10400000</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -887,19 +889,19 @@
         <v>10110000</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="G10">
         <v>99</v>
@@ -916,19 +918,19 @@
         <v>10110001</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="G11">
         <v>99</v>
@@ -945,19 +947,19 @@
         <v>10110002</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F12" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="G12">
         <v>99</v>
@@ -974,19 +976,19 @@
         <v>10110003</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F13" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="G13">
         <v>99</v>
@@ -1003,19 +1005,19 @@
         <v>10110004</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F14" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="G14">
         <v>99</v>
@@ -1038,7 +1040,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1049,25 +1051,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="F1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="G1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1218,8 +1220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAB882E2-DC2B-4364-A1E7-50F2FE65D6AC}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1234,22 +1236,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[Update] Player 스킬 UI 수정
</commit_message>
<xml_diff>
--- a/Assets/Resources/ItemData/ItemExcel.xlsx
+++ b/Assets/Resources/ItemData/ItemExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Unity\EscapeIsekai\Assets\Resources\ItemData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9460409-FC1D-458D-9228-B88FFAACDE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DD928C-3B34-4AF6-A3FA-05E66B8E3784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{23FCFA80-21D9-4745-B9DA-57060EA57FF8}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="173">
   <si>
     <t>나무 검</t>
   </si>
@@ -317,14 +317,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>포션 레시피</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>포션을 제작할 수 있습니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>나무로 만든 검입니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -507,10 +499,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>effect</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -564,6 +552,153 @@
   </si>
   <si>
     <t>hunger</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나무방패</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나무로 된 방배입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprite/Icon/Nomal_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>철방패</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>땅의 검</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빛의 검</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>불의 검</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아주 튼튼합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다루기에 큰 힘이 필요합니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가볍게 많이 휘두를 수 있습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>닿으면 많이 아플겁니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprite/Icon/Nomal_4</t>
+  </si>
+  <si>
+    <t>Sprite/Icon/Nomal_5</t>
+  </si>
+  <si>
+    <t>Sprite/Icon/Nomal_6</t>
+  </si>
+  <si>
+    <t>Sprite/Icon/Nomal_7</t>
+  </si>
+  <si>
+    <t>유물</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이것을 모아 현실로 돌아갑시다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprite/Icon/Nomal_0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빨간 포션을 제작할 수 있습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파란포션 레시피</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파란 포션을 제작할 수 있습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빨간 포션 레시피</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스테이크 레시피</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>브로콜리 레시피</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빵 레시피</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>닭다리 레시피</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카레 레시피</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>죽 레시피</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스프 레시피</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스테이크를 요리할 수 있습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>브로콜리를 요리할 수 있습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>닭다리를 요리할 수 있습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카레를 요리할 수 있습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스프를 요리할 수 있습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>죽을 요리할 수 있습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빵을 요리할 수 있습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprite/Icon/Nomal_1</t>
+  </si>
+  <si>
+    <t>Sprite/Icon/Nomal_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -928,10 +1063,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36525DF8-9879-4440-9A1B-CB7EE677C95C}">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -946,65 +1081,62 @@
     <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" t="s">
         <v>112</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>113</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>114</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>115</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>116</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>117</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>118</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>119</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>120</v>
       </c>
-      <c r="J1" t="s">
-        <v>121</v>
-      </c>
-      <c r="K1" t="s">
-        <v>122</v>
-      </c>
-      <c r="L1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>1001</v>
+        <v>16001</v>
       </c>
       <c r="B2" t="s">
         <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>156</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>153</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -1018,11 +1150,8 @@
       <c r="K2" t="b">
         <v>0</v>
       </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2001</v>
       </c>
@@ -1039,10 +1168,10 @@
         <v>100</v>
       </c>
       <c r="F3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H3">
         <v>99</v>
@@ -1056,11 +1185,8 @@
       <c r="K3" t="b">
         <v>1</v>
       </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2002</v>
       </c>
@@ -1077,10 +1203,10 @@
         <v>50</v>
       </c>
       <c r="F4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H4">
         <v>99</v>
@@ -1094,11 +1220,8 @@
       <c r="K4" t="b">
         <v>1</v>
       </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>2003</v>
       </c>
@@ -1115,10 +1238,10 @@
         <v>150</v>
       </c>
       <c r="F5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H5">
         <v>99</v>
@@ -1132,11 +1255,8 @@
       <c r="K5" t="b">
         <v>1</v>
       </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>2004</v>
       </c>
@@ -1153,10 +1273,10 @@
         <v>200</v>
       </c>
       <c r="F6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H6">
         <v>99</v>
@@ -1170,11 +1290,8 @@
       <c r="K6" t="b">
         <v>1</v>
       </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>2005</v>
       </c>
@@ -1191,10 +1308,10 @@
         <v>50</v>
       </c>
       <c r="F7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H7">
         <v>99</v>
@@ -1208,11 +1325,8 @@
       <c r="K7" t="b">
         <v>1</v>
       </c>
-      <c r="L7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>2006</v>
       </c>
@@ -1229,10 +1343,10 @@
         <v>100</v>
       </c>
       <c r="F8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H8">
         <v>99</v>
@@ -1246,11 +1360,8 @@
       <c r="K8" t="b">
         <v>1</v>
       </c>
-      <c r="L8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>2007</v>
       </c>
@@ -1267,10 +1378,10 @@
         <v>150</v>
       </c>
       <c r="F9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H9">
         <v>99</v>
@@ -1284,11 +1395,8 @@
       <c r="K9" t="b">
         <v>1</v>
       </c>
-      <c r="L9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>2008</v>
       </c>
@@ -1305,10 +1413,10 @@
         <v>100</v>
       </c>
       <c r="F10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H10">
         <v>99</v>
@@ -1322,11 +1430,8 @@
       <c r="K10" t="b">
         <v>1</v>
       </c>
-      <c r="L10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>3002</v>
       </c>
@@ -1343,10 +1448,10 @@
         <v>500</v>
       </c>
       <c r="F11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H11">
         <v>99</v>
@@ -1360,11 +1465,8 @@
       <c r="K11" t="b">
         <v>1</v>
       </c>
-      <c r="L11">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>3003</v>
       </c>
@@ -1381,10 +1483,10 @@
         <v>100</v>
       </c>
       <c r="F12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H12">
         <v>99</v>
@@ -1398,11 +1500,8 @@
       <c r="K12" t="b">
         <v>1</v>
       </c>
-      <c r="L12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>3004</v>
       </c>
@@ -1419,10 +1518,10 @@
         <v>200</v>
       </c>
       <c r="F13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H13">
         <v>99</v>
@@ -1436,11 +1535,8 @@
       <c r="K13" t="b">
         <v>1</v>
       </c>
-      <c r="L13">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>3006</v>
       </c>
@@ -1448,7 +1544,7 @@
         <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D14" t="s">
         <v>55</v>
@@ -1457,10 +1553,10 @@
         <v>300</v>
       </c>
       <c r="F14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H14">
         <v>99</v>
@@ -1474,11 +1570,8 @@
       <c r="K14" t="b">
         <v>1</v>
       </c>
-      <c r="L14">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>3007</v>
       </c>
@@ -1495,10 +1588,10 @@
         <v>700</v>
       </c>
       <c r="F15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H15">
         <v>99</v>
@@ -1512,11 +1605,8 @@
       <c r="K15" t="b">
         <v>1</v>
       </c>
-      <c r="L15">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>3008</v>
       </c>
@@ -1533,10 +1623,10 @@
         <v>500</v>
       </c>
       <c r="F16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H16">
         <v>99</v>
@@ -1550,11 +1640,8 @@
       <c r="K16" t="b">
         <v>1</v>
       </c>
-      <c r="L16">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>3009</v>
       </c>
@@ -1571,10 +1658,10 @@
         <v>600</v>
       </c>
       <c r="F17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G17" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H17">
         <v>99</v>
@@ -1588,11 +1675,8 @@
       <c r="K17" t="b">
         <v>1</v>
       </c>
-      <c r="L17">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>4101</v>
       </c>
@@ -1603,16 +1687,16 @@
         <v>72</v>
       </c>
       <c r="D18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E18">
         <v>1000</v>
       </c>
       <c r="F18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -1626,34 +1710,28 @@
       <c r="K18" t="b">
         <v>0</v>
       </c>
-      <c r="L18">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>6001</v>
+        <v>4102</v>
       </c>
       <c r="B19" t="s">
         <v>67</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>139</v>
       </c>
       <c r="D19" t="s">
-        <v>69</v>
+        <v>143</v>
       </c>
       <c r="E19">
-        <v>500</v>
-      </c>
-      <c r="F19" t="s">
-        <v>78</v>
+        <v>3000</v>
       </c>
       <c r="G19" t="s">
-        <v>110</v>
+        <v>147</v>
       </c>
       <c r="H19">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="I19" t="b">
         <v>1</v>
@@ -1664,402 +1742,357 @@
       <c r="K19" t="b">
         <v>1</v>
       </c>
-      <c r="L19">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20">
-        <v>6002</v>
+        <v>4103</v>
       </c>
       <c r="B20" t="s">
         <v>67</v>
       </c>
       <c r="C20" t="s">
+        <v>140</v>
+      </c>
+      <c r="D20" t="s">
+        <v>144</v>
+      </c>
+      <c r="E20">
+        <v>4000</v>
+      </c>
+      <c r="G20" t="s">
+        <v>148</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>4104</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
+        <v>141</v>
+      </c>
+      <c r="D21" t="s">
+        <v>145</v>
+      </c>
+      <c r="E21">
+        <v>5000</v>
+      </c>
+      <c r="G21" t="s">
+        <v>149</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>4201</v>
+      </c>
+      <c r="B22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" t="s">
+        <v>135</v>
+      </c>
+      <c r="D22" t="s">
+        <v>136</v>
+      </c>
+      <c r="E22">
+        <v>1000</v>
+      </c>
+      <c r="G22" t="s">
+        <v>137</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>4202</v>
+      </c>
+      <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" t="s">
+        <v>138</v>
+      </c>
+      <c r="D23" t="s">
+        <v>142</v>
+      </c>
+      <c r="E23">
+        <v>2000</v>
+      </c>
+      <c r="G23" t="s">
+        <v>146</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J23" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>6001</v>
+      </c>
+      <c r="B24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24">
+        <v>500</v>
+      </c>
+      <c r="F24" t="s">
+        <v>76</v>
+      </c>
+      <c r="G24" t="s">
+        <v>108</v>
+      </c>
+      <c r="H24">
+        <v>99</v>
+      </c>
+      <c r="I24" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>6002</v>
+      </c>
+      <c r="B25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" t="s">
         <v>70</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D25" t="s">
         <v>71</v>
       </c>
-      <c r="E20">
+      <c r="E25">
         <v>500</v>
       </c>
-      <c r="F20" t="s">
-        <v>78</v>
-      </c>
-      <c r="G20" t="s">
-        <v>111</v>
-      </c>
-      <c r="H20">
-        <v>99</v>
-      </c>
-      <c r="I20" t="b">
-        <v>0</v>
-      </c>
-      <c r="J20" t="b">
-        <v>0</v>
-      </c>
-      <c r="K20" t="b">
-        <v>1</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A21">
-        <v>10000000</v>
-      </c>
-      <c r="B21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21">
-        <v>10</v>
-      </c>
-      <c r="F21" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" t="s">
-        <v>29</v>
-      </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-      <c r="I21" t="b">
-        <v>1</v>
-      </c>
-      <c r="J21" t="b">
-        <v>1</v>
-      </c>
-      <c r="K21" t="b">
-        <v>1</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A22">
-        <v>10001000</v>
-      </c>
-      <c r="B22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22">
-        <v>10</v>
-      </c>
-      <c r="F22" t="s">
-        <v>15</v>
-      </c>
-      <c r="G22" t="s">
-        <v>29</v>
-      </c>
-      <c r="H22">
-        <v>1</v>
-      </c>
-      <c r="I22" t="b">
-        <v>1</v>
-      </c>
-      <c r="J22" t="b">
-        <v>1</v>
-      </c>
-      <c r="K22" t="b">
-        <v>1</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A23">
-        <v>10002000</v>
-      </c>
-      <c r="B23" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23">
-        <v>10</v>
-      </c>
-      <c r="F23" t="s">
-        <v>15</v>
-      </c>
-      <c r="G23" t="s">
-        <v>29</v>
-      </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-      <c r="I23" t="b">
-        <v>1</v>
-      </c>
-      <c r="J23" t="b">
-        <v>1</v>
-      </c>
-      <c r="K23" t="b">
-        <v>1</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A24">
-        <v>10010000</v>
-      </c>
-      <c r="B24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" t="s">
-        <v>0</v>
-      </c>
-      <c r="D24" t="s">
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <v>10</v>
-      </c>
-      <c r="F24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G24" t="s">
-        <v>18</v>
-      </c>
-      <c r="H24">
-        <v>1</v>
-      </c>
-      <c r="I24" t="b">
-        <v>1</v>
-      </c>
-      <c r="J24" t="b">
-        <v>1</v>
-      </c>
-      <c r="K24" t="b">
-        <v>1</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A25">
-        <v>10100000</v>
-      </c>
-      <c r="B25" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
       <c r="F25" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="G25" t="s">
-        <v>31</v>
+        <v>109</v>
       </c>
       <c r="H25">
         <v>99</v>
       </c>
       <c r="I25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K25" t="b">
         <v>1</v>
       </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>10110000</v>
+        <v>10000000</v>
       </c>
       <c r="B26" t="s">
         <v>35</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F26" t="s">
         <v>15</v>
       </c>
       <c r="G26" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H26">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="I26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" t="b">
         <v>1</v>
       </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27">
-        <v>10110001</v>
+        <v>10001000</v>
       </c>
       <c r="B27" t="s">
         <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F27" t="s">
         <v>15</v>
       </c>
       <c r="G27" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H27">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="I27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" t="b">
         <v>1</v>
       </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28">
-        <v>10110002</v>
+        <v>10002000</v>
       </c>
       <c r="B28" t="s">
         <v>35</v>
       </c>
       <c r="C28" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F28" t="s">
         <v>15</v>
       </c>
       <c r="G28" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H28">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="I28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28" t="b">
         <v>1</v>
       </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29">
-        <v>10110003</v>
+        <v>10010000</v>
       </c>
       <c r="B29" t="s">
         <v>35</v>
       </c>
       <c r="C29" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F29" t="s">
         <v>15</v>
       </c>
       <c r="G29" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="H29">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="I29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K29" t="b">
         <v>1</v>
       </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30">
-        <v>10110004</v>
+        <v>10100000</v>
       </c>
       <c r="B30" t="s">
         <v>35</v>
       </c>
       <c r="C30" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D30" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -2068,48 +2101,45 @@
         <v>15</v>
       </c>
       <c r="G30" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H30">
         <v>99</v>
       </c>
       <c r="I30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K30" t="b">
         <v>1</v>
       </c>
-      <c r="L30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31">
-        <v>10200000</v>
+        <v>10110000</v>
       </c>
       <c r="B31" t="s">
         <v>35</v>
       </c>
       <c r="C31" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="D31" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="E31">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G31" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="H31">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="I31" t="b">
         <v>0</v>
@@ -2120,31 +2150,28 @@
       <c r="K31" t="b">
         <v>1</v>
       </c>
-      <c r="L31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32">
-        <v>10300000</v>
+        <v>10110001</v>
       </c>
       <c r="B32" t="s">
         <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D32" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E32">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F32" t="s">
         <v>15</v>
       </c>
       <c r="G32" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H32">
         <v>99</v>
@@ -2158,22 +2185,19 @@
       <c r="K32" t="b">
         <v>1</v>
       </c>
-      <c r="L32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33">
-        <v>10400000</v>
+        <v>10110002</v>
       </c>
       <c r="B33" t="s">
         <v>35</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D33" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -2182,27 +2206,523 @@
         <v>15</v>
       </c>
       <c r="G33" t="s">
+        <v>33</v>
+      </c>
+      <c r="H33">
+        <v>99</v>
+      </c>
+      <c r="I33" t="b">
+        <v>0</v>
+      </c>
+      <c r="J33" t="b">
+        <v>0</v>
+      </c>
+      <c r="K33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>10110003</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H34">
+        <v>99</v>
+      </c>
+      <c r="I34" t="b">
+        <v>0</v>
+      </c>
+      <c r="J34" t="b">
+        <v>0</v>
+      </c>
+      <c r="K34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>10110004</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35" t="s">
+        <v>15</v>
+      </c>
+      <c r="G35" t="s">
+        <v>34</v>
+      </c>
+      <c r="H35">
+        <v>99</v>
+      </c>
+      <c r="I35" t="b">
+        <v>0</v>
+      </c>
+      <c r="J35" t="b">
+        <v>0</v>
+      </c>
+      <c r="K35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>10200000</v>
+      </c>
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <v>10</v>
+      </c>
+      <c r="F36" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36" t="b">
+        <v>0</v>
+      </c>
+      <c r="J36" t="b">
+        <v>0</v>
+      </c>
+      <c r="K36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>10300000</v>
+      </c>
+      <c r="B37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37">
+        <v>100</v>
+      </c>
+      <c r="F37" t="s">
+        <v>15</v>
+      </c>
+      <c r="G37" t="s">
         <v>30</v>
       </c>
-      <c r="H33">
-        <v>1</v>
-      </c>
-      <c r="I33" t="b">
-        <v>1</v>
-      </c>
-      <c r="J33" t="b">
-        <v>0</v>
-      </c>
-      <c r="K33" t="b">
-        <v>1</v>
-      </c>
-      <c r="L33">
-        <v>0</v>
+      <c r="H37">
+        <v>99</v>
+      </c>
+      <c r="I37" t="b">
+        <v>0</v>
+      </c>
+      <c r="J37" t="b">
+        <v>0</v>
+      </c>
+      <c r="K37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>10400000</v>
+      </c>
+      <c r="B38" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" t="s">
+        <v>15</v>
+      </c>
+      <c r="G38" t="s">
+        <v>30</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38" t="b">
+        <v>1</v>
+      </c>
+      <c r="J38" t="b">
+        <v>0</v>
+      </c>
+      <c r="K38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>5000</v>
+      </c>
+      <c r="B39" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" t="s">
+        <v>150</v>
+      </c>
+      <c r="D39" t="s">
+        <v>151</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="G39" t="s">
+        <v>152</v>
+      </c>
+      <c r="H39">
+        <v>4</v>
+      </c>
+      <c r="I39" t="b">
+        <v>0</v>
+      </c>
+      <c r="J39" t="b">
+        <v>0</v>
+      </c>
+      <c r="K39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>16002</v>
+      </c>
+      <c r="B40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" t="s">
+        <v>154</v>
+      </c>
+      <c r="D40" t="s">
+        <v>155</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40" t="s">
+        <v>75</v>
+      </c>
+      <c r="G40" t="s">
+        <v>92</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40" t="b">
+        <v>0</v>
+      </c>
+      <c r="J40" t="b">
+        <v>1</v>
+      </c>
+      <c r="K40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>13002</v>
+      </c>
+      <c r="B41" t="s">
+        <v>35</v>
+      </c>
+      <c r="C41" t="s">
+        <v>157</v>
+      </c>
+      <c r="D41" t="s">
+        <v>164</v>
+      </c>
+      <c r="F41" t="s">
+        <v>75</v>
+      </c>
+      <c r="G41" t="s">
+        <v>172</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41" t="b">
+        <v>0</v>
+      </c>
+      <c r="J41" t="b">
+        <v>1</v>
+      </c>
+      <c r="K41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>13003</v>
+      </c>
+      <c r="B42" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" t="s">
+        <v>158</v>
+      </c>
+      <c r="D42" t="s">
+        <v>165</v>
+      </c>
+      <c r="F42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G42" t="s">
+        <v>171</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42" t="b">
+        <v>0</v>
+      </c>
+      <c r="J42" t="b">
+        <v>1</v>
+      </c>
+      <c r="K42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>13004</v>
+      </c>
+      <c r="B43" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" t="s">
+        <v>159</v>
+      </c>
+      <c r="D43" t="s">
+        <v>170</v>
+      </c>
+      <c r="F43" t="s">
+        <v>75</v>
+      </c>
+      <c r="G43" t="s">
+        <v>171</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43" t="b">
+        <v>0</v>
+      </c>
+      <c r="J43" t="b">
+        <v>1</v>
+      </c>
+      <c r="K43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>13005</v>
+      </c>
+      <c r="B44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" t="s">
+        <v>160</v>
+      </c>
+      <c r="D44" t="s">
+        <v>166</v>
+      </c>
+      <c r="F44" t="s">
+        <v>75</v>
+      </c>
+      <c r="G44" t="s">
+        <v>171</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44" t="b">
+        <v>0</v>
+      </c>
+      <c r="J44" t="b">
+        <v>1</v>
+      </c>
+      <c r="K44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>13006</v>
+      </c>
+      <c r="B45" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" t="s">
+        <v>161</v>
+      </c>
+      <c r="D45" t="s">
+        <v>167</v>
+      </c>
+      <c r="F45" t="s">
+        <v>75</v>
+      </c>
+      <c r="G45" t="s">
+        <v>171</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="I45" t="b">
+        <v>0</v>
+      </c>
+      <c r="J45" t="b">
+        <v>1</v>
+      </c>
+      <c r="K45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>13007</v>
+      </c>
+      <c r="B46" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" t="s">
+        <v>162</v>
+      </c>
+      <c r="D46" t="s">
+        <v>169</v>
+      </c>
+      <c r="F46" t="s">
+        <v>75</v>
+      </c>
+      <c r="G46" t="s">
+        <v>171</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46" t="b">
+        <v>0</v>
+      </c>
+      <c r="J46" t="b">
+        <v>1</v>
+      </c>
+      <c r="K46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>13008</v>
+      </c>
+      <c r="B47" t="s">
+        <v>35</v>
+      </c>
+      <c r="C47" t="s">
+        <v>163</v>
+      </c>
+      <c r="D47" t="s">
+        <v>168</v>
+      </c>
+      <c r="F47" t="s">
+        <v>75</v>
+      </c>
+      <c r="G47" t="s">
+        <v>171</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="I47" t="b">
+        <v>0</v>
+      </c>
+      <c r="J47" t="b">
+        <v>1</v>
+      </c>
+      <c r="K47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>1401</v>
+      </c>
+      <c r="C48" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C49" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C50" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C51" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C52" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C53" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L33">
-    <sortCondition ref="A33"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K38">
+    <sortCondition ref="A2:A38"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2211,10 +2731,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{046DC669-D6D6-48C0-9A46-A8FD3A6BBB2C}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2225,28 +2745,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" t="s">
         <v>124</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>125</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>126</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>127</v>
       </c>
-      <c r="E1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G1" t="s">
-        <v>130</v>
-      </c>
       <c r="H1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
@@ -2740,6 +3260,136 @@
         <v>0</v>
       </c>
       <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>4201</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>30</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>4202</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>80</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>4102</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>50</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>4103</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>70</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>4104</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>80</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
         <v>0</v>
       </c>
     </row>
@@ -2769,22 +3419,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" t="s">
         <v>131</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>132</v>
-      </c>
-      <c r="D1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Shj/shj end scene (#66)
* [Update] DayNight UI 디자인 수정

* [Add] EndScene 시나리오 연출 제작

* [Add] EndScene Credit추가

* [Update] player UI디자인 수정

* [Update] Player 스킬 UI 수정
</commit_message>
<xml_diff>
--- a/Assets/Resources/ItemData/ItemExcel.xlsx
+++ b/Assets/Resources/ItemData/ItemExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Unity\EscapeIsekai\Assets\Resources\ItemData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9460409-FC1D-458D-9228-B88FFAACDE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DD928C-3B34-4AF6-A3FA-05E66B8E3784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{23FCFA80-21D9-4745-B9DA-57060EA57FF8}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="173">
   <si>
     <t>나무 검</t>
   </si>
@@ -317,14 +317,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>포션 레시피</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>포션을 제작할 수 있습니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>나무로 만든 검입니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -507,10 +499,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>effect</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -564,6 +552,153 @@
   </si>
   <si>
     <t>hunger</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나무방패</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나무로 된 방배입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprite/Icon/Nomal_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>철방패</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>땅의 검</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빛의 검</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>불의 검</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아주 튼튼합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다루기에 큰 힘이 필요합니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가볍게 많이 휘두를 수 있습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>닿으면 많이 아플겁니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprite/Icon/Nomal_4</t>
+  </si>
+  <si>
+    <t>Sprite/Icon/Nomal_5</t>
+  </si>
+  <si>
+    <t>Sprite/Icon/Nomal_6</t>
+  </si>
+  <si>
+    <t>Sprite/Icon/Nomal_7</t>
+  </si>
+  <si>
+    <t>유물</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이것을 모아 현실로 돌아갑시다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprite/Icon/Nomal_0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빨간 포션을 제작할 수 있습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파란포션 레시피</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파란 포션을 제작할 수 있습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빨간 포션 레시피</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스테이크 레시피</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>브로콜리 레시피</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빵 레시피</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>닭다리 레시피</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카레 레시피</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>죽 레시피</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스프 레시피</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스테이크를 요리할 수 있습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>브로콜리를 요리할 수 있습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>닭다리를 요리할 수 있습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카레를 요리할 수 있습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스프를 요리할 수 있습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>죽을 요리할 수 있습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빵을 요리할 수 있습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprite/Icon/Nomal_1</t>
+  </si>
+  <si>
+    <t>Sprite/Icon/Nomal_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -928,10 +1063,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36525DF8-9879-4440-9A1B-CB7EE677C95C}">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -946,65 +1081,62 @@
     <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" t="s">
         <v>112</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>113</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>114</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>115</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>116</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>117</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>118</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>119</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>120</v>
       </c>
-      <c r="J1" t="s">
-        <v>121</v>
-      </c>
-      <c r="K1" t="s">
-        <v>122</v>
-      </c>
-      <c r="L1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>1001</v>
+        <v>16001</v>
       </c>
       <c r="B2" t="s">
         <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>156</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>153</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -1018,11 +1150,8 @@
       <c r="K2" t="b">
         <v>0</v>
       </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2001</v>
       </c>
@@ -1039,10 +1168,10 @@
         <v>100</v>
       </c>
       <c r="F3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H3">
         <v>99</v>
@@ -1056,11 +1185,8 @@
       <c r="K3" t="b">
         <v>1</v>
       </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2002</v>
       </c>
@@ -1077,10 +1203,10 @@
         <v>50</v>
       </c>
       <c r="F4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H4">
         <v>99</v>
@@ -1094,11 +1220,8 @@
       <c r="K4" t="b">
         <v>1</v>
       </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>2003</v>
       </c>
@@ -1115,10 +1238,10 @@
         <v>150</v>
       </c>
       <c r="F5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H5">
         <v>99</v>
@@ -1132,11 +1255,8 @@
       <c r="K5" t="b">
         <v>1</v>
       </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>2004</v>
       </c>
@@ -1153,10 +1273,10 @@
         <v>200</v>
       </c>
       <c r="F6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H6">
         <v>99</v>
@@ -1170,11 +1290,8 @@
       <c r="K6" t="b">
         <v>1</v>
       </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>2005</v>
       </c>
@@ -1191,10 +1308,10 @@
         <v>50</v>
       </c>
       <c r="F7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H7">
         <v>99</v>
@@ -1208,11 +1325,8 @@
       <c r="K7" t="b">
         <v>1</v>
       </c>
-      <c r="L7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>2006</v>
       </c>
@@ -1229,10 +1343,10 @@
         <v>100</v>
       </c>
       <c r="F8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H8">
         <v>99</v>
@@ -1246,11 +1360,8 @@
       <c r="K8" t="b">
         <v>1</v>
       </c>
-      <c r="L8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>2007</v>
       </c>
@@ -1267,10 +1378,10 @@
         <v>150</v>
       </c>
       <c r="F9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H9">
         <v>99</v>
@@ -1284,11 +1395,8 @@
       <c r="K9" t="b">
         <v>1</v>
       </c>
-      <c r="L9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>2008</v>
       </c>
@@ -1305,10 +1413,10 @@
         <v>100</v>
       </c>
       <c r="F10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H10">
         <v>99</v>
@@ -1322,11 +1430,8 @@
       <c r="K10" t="b">
         <v>1</v>
       </c>
-      <c r="L10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>3002</v>
       </c>
@@ -1343,10 +1448,10 @@
         <v>500</v>
       </c>
       <c r="F11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H11">
         <v>99</v>
@@ -1360,11 +1465,8 @@
       <c r="K11" t="b">
         <v>1</v>
       </c>
-      <c r="L11">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>3003</v>
       </c>
@@ -1381,10 +1483,10 @@
         <v>100</v>
       </c>
       <c r="F12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H12">
         <v>99</v>
@@ -1398,11 +1500,8 @@
       <c r="K12" t="b">
         <v>1</v>
       </c>
-      <c r="L12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>3004</v>
       </c>
@@ -1419,10 +1518,10 @@
         <v>200</v>
       </c>
       <c r="F13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H13">
         <v>99</v>
@@ -1436,11 +1535,8 @@
       <c r="K13" t="b">
         <v>1</v>
       </c>
-      <c r="L13">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>3006</v>
       </c>
@@ -1448,7 +1544,7 @@
         <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D14" t="s">
         <v>55</v>
@@ -1457,10 +1553,10 @@
         <v>300</v>
       </c>
       <c r="F14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H14">
         <v>99</v>
@@ -1474,11 +1570,8 @@
       <c r="K14" t="b">
         <v>1</v>
       </c>
-      <c r="L14">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>3007</v>
       </c>
@@ -1495,10 +1588,10 @@
         <v>700</v>
       </c>
       <c r="F15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H15">
         <v>99</v>
@@ -1512,11 +1605,8 @@
       <c r="K15" t="b">
         <v>1</v>
       </c>
-      <c r="L15">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>3008</v>
       </c>
@@ -1533,10 +1623,10 @@
         <v>500</v>
       </c>
       <c r="F16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H16">
         <v>99</v>
@@ -1550,11 +1640,8 @@
       <c r="K16" t="b">
         <v>1</v>
       </c>
-      <c r="L16">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>3009</v>
       </c>
@@ -1571,10 +1658,10 @@
         <v>600</v>
       </c>
       <c r="F17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G17" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H17">
         <v>99</v>
@@ -1588,11 +1675,8 @@
       <c r="K17" t="b">
         <v>1</v>
       </c>
-      <c r="L17">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>4101</v>
       </c>
@@ -1603,16 +1687,16 @@
         <v>72</v>
       </c>
       <c r="D18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E18">
         <v>1000</v>
       </c>
       <c r="F18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -1626,34 +1710,28 @@
       <c r="K18" t="b">
         <v>0</v>
       </c>
-      <c r="L18">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>6001</v>
+        <v>4102</v>
       </c>
       <c r="B19" t="s">
         <v>67</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>139</v>
       </c>
       <c r="D19" t="s">
-        <v>69</v>
+        <v>143</v>
       </c>
       <c r="E19">
-        <v>500</v>
-      </c>
-      <c r="F19" t="s">
-        <v>78</v>
+        <v>3000</v>
       </c>
       <c r="G19" t="s">
-        <v>110</v>
+        <v>147</v>
       </c>
       <c r="H19">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="I19" t="b">
         <v>1</v>
@@ -1664,402 +1742,357 @@
       <c r="K19" t="b">
         <v>1</v>
       </c>
-      <c r="L19">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20">
-        <v>6002</v>
+        <v>4103</v>
       </c>
       <c r="B20" t="s">
         <v>67</v>
       </c>
       <c r="C20" t="s">
+        <v>140</v>
+      </c>
+      <c r="D20" t="s">
+        <v>144</v>
+      </c>
+      <c r="E20">
+        <v>4000</v>
+      </c>
+      <c r="G20" t="s">
+        <v>148</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>4104</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
+        <v>141</v>
+      </c>
+      <c r="D21" t="s">
+        <v>145</v>
+      </c>
+      <c r="E21">
+        <v>5000</v>
+      </c>
+      <c r="G21" t="s">
+        <v>149</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>4201</v>
+      </c>
+      <c r="B22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" t="s">
+        <v>135</v>
+      </c>
+      <c r="D22" t="s">
+        <v>136</v>
+      </c>
+      <c r="E22">
+        <v>1000</v>
+      </c>
+      <c r="G22" t="s">
+        <v>137</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>4202</v>
+      </c>
+      <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" t="s">
+        <v>138</v>
+      </c>
+      <c r="D23" t="s">
+        <v>142</v>
+      </c>
+      <c r="E23">
+        <v>2000</v>
+      </c>
+      <c r="G23" t="s">
+        <v>146</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J23" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>6001</v>
+      </c>
+      <c r="B24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24">
+        <v>500</v>
+      </c>
+      <c r="F24" t="s">
+        <v>76</v>
+      </c>
+      <c r="G24" t="s">
+        <v>108</v>
+      </c>
+      <c r="H24">
+        <v>99</v>
+      </c>
+      <c r="I24" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>6002</v>
+      </c>
+      <c r="B25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" t="s">
         <v>70</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D25" t="s">
         <v>71</v>
       </c>
-      <c r="E20">
+      <c r="E25">
         <v>500</v>
       </c>
-      <c r="F20" t="s">
-        <v>78</v>
-      </c>
-      <c r="G20" t="s">
-        <v>111</v>
-      </c>
-      <c r="H20">
-        <v>99</v>
-      </c>
-      <c r="I20" t="b">
-        <v>0</v>
-      </c>
-      <c r="J20" t="b">
-        <v>0</v>
-      </c>
-      <c r="K20" t="b">
-        <v>1</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A21">
-        <v>10000000</v>
-      </c>
-      <c r="B21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21">
-        <v>10</v>
-      </c>
-      <c r="F21" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" t="s">
-        <v>29</v>
-      </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-      <c r="I21" t="b">
-        <v>1</v>
-      </c>
-      <c r="J21" t="b">
-        <v>1</v>
-      </c>
-      <c r="K21" t="b">
-        <v>1</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A22">
-        <v>10001000</v>
-      </c>
-      <c r="B22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22">
-        <v>10</v>
-      </c>
-      <c r="F22" t="s">
-        <v>15</v>
-      </c>
-      <c r="G22" t="s">
-        <v>29</v>
-      </c>
-      <c r="H22">
-        <v>1</v>
-      </c>
-      <c r="I22" t="b">
-        <v>1</v>
-      </c>
-      <c r="J22" t="b">
-        <v>1</v>
-      </c>
-      <c r="K22" t="b">
-        <v>1</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A23">
-        <v>10002000</v>
-      </c>
-      <c r="B23" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23">
-        <v>10</v>
-      </c>
-      <c r="F23" t="s">
-        <v>15</v>
-      </c>
-      <c r="G23" t="s">
-        <v>29</v>
-      </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-      <c r="I23" t="b">
-        <v>1</v>
-      </c>
-      <c r="J23" t="b">
-        <v>1</v>
-      </c>
-      <c r="K23" t="b">
-        <v>1</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A24">
-        <v>10010000</v>
-      </c>
-      <c r="B24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" t="s">
-        <v>0</v>
-      </c>
-      <c r="D24" t="s">
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <v>10</v>
-      </c>
-      <c r="F24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G24" t="s">
-        <v>18</v>
-      </c>
-      <c r="H24">
-        <v>1</v>
-      </c>
-      <c r="I24" t="b">
-        <v>1</v>
-      </c>
-      <c r="J24" t="b">
-        <v>1</v>
-      </c>
-      <c r="K24" t="b">
-        <v>1</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A25">
-        <v>10100000</v>
-      </c>
-      <c r="B25" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
       <c r="F25" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="G25" t="s">
-        <v>31</v>
+        <v>109</v>
       </c>
       <c r="H25">
         <v>99</v>
       </c>
       <c r="I25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K25" t="b">
         <v>1</v>
       </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>10110000</v>
+        <v>10000000</v>
       </c>
       <c r="B26" t="s">
         <v>35</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F26" t="s">
         <v>15</v>
       </c>
       <c r="G26" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H26">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="I26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" t="b">
         <v>1</v>
       </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27">
-        <v>10110001</v>
+        <v>10001000</v>
       </c>
       <c r="B27" t="s">
         <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F27" t="s">
         <v>15</v>
       </c>
       <c r="G27" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H27">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="I27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" t="b">
         <v>1</v>
       </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28">
-        <v>10110002</v>
+        <v>10002000</v>
       </c>
       <c r="B28" t="s">
         <v>35</v>
       </c>
       <c r="C28" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F28" t="s">
         <v>15</v>
       </c>
       <c r="G28" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H28">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="I28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28" t="b">
         <v>1</v>
       </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29">
-        <v>10110003</v>
+        <v>10010000</v>
       </c>
       <c r="B29" t="s">
         <v>35</v>
       </c>
       <c r="C29" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F29" t="s">
         <v>15</v>
       </c>
       <c r="G29" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="H29">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="I29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K29" t="b">
         <v>1</v>
       </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30">
-        <v>10110004</v>
+        <v>10100000</v>
       </c>
       <c r="B30" t="s">
         <v>35</v>
       </c>
       <c r="C30" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D30" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -2068,48 +2101,45 @@
         <v>15</v>
       </c>
       <c r="G30" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H30">
         <v>99</v>
       </c>
       <c r="I30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K30" t="b">
         <v>1</v>
       </c>
-      <c r="L30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31">
-        <v>10200000</v>
+        <v>10110000</v>
       </c>
       <c r="B31" t="s">
         <v>35</v>
       </c>
       <c r="C31" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="D31" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="E31">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G31" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="H31">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="I31" t="b">
         <v>0</v>
@@ -2120,31 +2150,28 @@
       <c r="K31" t="b">
         <v>1</v>
       </c>
-      <c r="L31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32">
-        <v>10300000</v>
+        <v>10110001</v>
       </c>
       <c r="B32" t="s">
         <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D32" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E32">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F32" t="s">
         <v>15</v>
       </c>
       <c r="G32" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H32">
         <v>99</v>
@@ -2158,22 +2185,19 @@
       <c r="K32" t="b">
         <v>1</v>
       </c>
-      <c r="L32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33">
-        <v>10400000</v>
+        <v>10110002</v>
       </c>
       <c r="B33" t="s">
         <v>35</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D33" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -2182,27 +2206,523 @@
         <v>15</v>
       </c>
       <c r="G33" t="s">
+        <v>33</v>
+      </c>
+      <c r="H33">
+        <v>99</v>
+      </c>
+      <c r="I33" t="b">
+        <v>0</v>
+      </c>
+      <c r="J33" t="b">
+        <v>0</v>
+      </c>
+      <c r="K33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>10110003</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H34">
+        <v>99</v>
+      </c>
+      <c r="I34" t="b">
+        <v>0</v>
+      </c>
+      <c r="J34" t="b">
+        <v>0</v>
+      </c>
+      <c r="K34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>10110004</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35" t="s">
+        <v>15</v>
+      </c>
+      <c r="G35" t="s">
+        <v>34</v>
+      </c>
+      <c r="H35">
+        <v>99</v>
+      </c>
+      <c r="I35" t="b">
+        <v>0</v>
+      </c>
+      <c r="J35" t="b">
+        <v>0</v>
+      </c>
+      <c r="K35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>10200000</v>
+      </c>
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <v>10</v>
+      </c>
+      <c r="F36" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36" t="b">
+        <v>0</v>
+      </c>
+      <c r="J36" t="b">
+        <v>0</v>
+      </c>
+      <c r="K36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>10300000</v>
+      </c>
+      <c r="B37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37">
+        <v>100</v>
+      </c>
+      <c r="F37" t="s">
+        <v>15</v>
+      </c>
+      <c r="G37" t="s">
         <v>30</v>
       </c>
-      <c r="H33">
-        <v>1</v>
-      </c>
-      <c r="I33" t="b">
-        <v>1</v>
-      </c>
-      <c r="J33" t="b">
-        <v>0</v>
-      </c>
-      <c r="K33" t="b">
-        <v>1</v>
-      </c>
-      <c r="L33">
-        <v>0</v>
+      <c r="H37">
+        <v>99</v>
+      </c>
+      <c r="I37" t="b">
+        <v>0</v>
+      </c>
+      <c r="J37" t="b">
+        <v>0</v>
+      </c>
+      <c r="K37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>10400000</v>
+      </c>
+      <c r="B38" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" t="s">
+        <v>15</v>
+      </c>
+      <c r="G38" t="s">
+        <v>30</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38" t="b">
+        <v>1</v>
+      </c>
+      <c r="J38" t="b">
+        <v>0</v>
+      </c>
+      <c r="K38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>5000</v>
+      </c>
+      <c r="B39" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" t="s">
+        <v>150</v>
+      </c>
+      <c r="D39" t="s">
+        <v>151</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="G39" t="s">
+        <v>152</v>
+      </c>
+      <c r="H39">
+        <v>4</v>
+      </c>
+      <c r="I39" t="b">
+        <v>0</v>
+      </c>
+      <c r="J39" t="b">
+        <v>0</v>
+      </c>
+      <c r="K39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>16002</v>
+      </c>
+      <c r="B40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" t="s">
+        <v>154</v>
+      </c>
+      <c r="D40" t="s">
+        <v>155</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40" t="s">
+        <v>75</v>
+      </c>
+      <c r="G40" t="s">
+        <v>92</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40" t="b">
+        <v>0</v>
+      </c>
+      <c r="J40" t="b">
+        <v>1</v>
+      </c>
+      <c r="K40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>13002</v>
+      </c>
+      <c r="B41" t="s">
+        <v>35</v>
+      </c>
+      <c r="C41" t="s">
+        <v>157</v>
+      </c>
+      <c r="D41" t="s">
+        <v>164</v>
+      </c>
+      <c r="F41" t="s">
+        <v>75</v>
+      </c>
+      <c r="G41" t="s">
+        <v>172</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41" t="b">
+        <v>0</v>
+      </c>
+      <c r="J41" t="b">
+        <v>1</v>
+      </c>
+      <c r="K41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>13003</v>
+      </c>
+      <c r="B42" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" t="s">
+        <v>158</v>
+      </c>
+      <c r="D42" t="s">
+        <v>165</v>
+      </c>
+      <c r="F42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G42" t="s">
+        <v>171</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42" t="b">
+        <v>0</v>
+      </c>
+      <c r="J42" t="b">
+        <v>1</v>
+      </c>
+      <c r="K42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>13004</v>
+      </c>
+      <c r="B43" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" t="s">
+        <v>159</v>
+      </c>
+      <c r="D43" t="s">
+        <v>170</v>
+      </c>
+      <c r="F43" t="s">
+        <v>75</v>
+      </c>
+      <c r="G43" t="s">
+        <v>171</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43" t="b">
+        <v>0</v>
+      </c>
+      <c r="J43" t="b">
+        <v>1</v>
+      </c>
+      <c r="K43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>13005</v>
+      </c>
+      <c r="B44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" t="s">
+        <v>160</v>
+      </c>
+      <c r="D44" t="s">
+        <v>166</v>
+      </c>
+      <c r="F44" t="s">
+        <v>75</v>
+      </c>
+      <c r="G44" t="s">
+        <v>171</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44" t="b">
+        <v>0</v>
+      </c>
+      <c r="J44" t="b">
+        <v>1</v>
+      </c>
+      <c r="K44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>13006</v>
+      </c>
+      <c r="B45" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" t="s">
+        <v>161</v>
+      </c>
+      <c r="D45" t="s">
+        <v>167</v>
+      </c>
+      <c r="F45" t="s">
+        <v>75</v>
+      </c>
+      <c r="G45" t="s">
+        <v>171</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="I45" t="b">
+        <v>0</v>
+      </c>
+      <c r="J45" t="b">
+        <v>1</v>
+      </c>
+      <c r="K45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>13007</v>
+      </c>
+      <c r="B46" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" t="s">
+        <v>162</v>
+      </c>
+      <c r="D46" t="s">
+        <v>169</v>
+      </c>
+      <c r="F46" t="s">
+        <v>75</v>
+      </c>
+      <c r="G46" t="s">
+        <v>171</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46" t="b">
+        <v>0</v>
+      </c>
+      <c r="J46" t="b">
+        <v>1</v>
+      </c>
+      <c r="K46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>13008</v>
+      </c>
+      <c r="B47" t="s">
+        <v>35</v>
+      </c>
+      <c r="C47" t="s">
+        <v>163</v>
+      </c>
+      <c r="D47" t="s">
+        <v>168</v>
+      </c>
+      <c r="F47" t="s">
+        <v>75</v>
+      </c>
+      <c r="G47" t="s">
+        <v>171</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="I47" t="b">
+        <v>0</v>
+      </c>
+      <c r="J47" t="b">
+        <v>1</v>
+      </c>
+      <c r="K47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>1401</v>
+      </c>
+      <c r="C48" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C49" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C50" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C51" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C52" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C53" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L33">
-    <sortCondition ref="A33"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K38">
+    <sortCondition ref="A2:A38"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2211,10 +2731,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{046DC669-D6D6-48C0-9A46-A8FD3A6BBB2C}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2225,28 +2745,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" t="s">
         <v>124</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>125</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>126</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>127</v>
       </c>
-      <c r="E1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G1" t="s">
-        <v>130</v>
-      </c>
       <c r="H1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
@@ -2740,6 +3260,136 @@
         <v>0</v>
       </c>
       <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>4201</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>30</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>4202</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>80</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>4102</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>50</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>4103</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>70</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>4104</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>80</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
         <v>0</v>
       </c>
     </row>
@@ -2769,22 +3419,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" t="s">
         <v>131</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>132</v>
-      </c>
-      <c r="D1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
[FIX]Trading UI And MainScene 기믹 설정 수정
</commit_message>
<xml_diff>
--- a/Assets/Resources/ItemData/ItemExcel.xlsx
+++ b/Assets/Resources/ItemData/ItemExcel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Unity\EscapeIsekai\Assets\Resources\ItemData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity\Team\EscapeIsekai\Assets\Resources\ItemData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32380F1A-6EAB-485C-9E9D-35D6F4630B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4C086E-03E5-44C5-BB4D-6CA00611F8CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{23FCFA80-21D9-4745-B9DA-57060EA57FF8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{23FCFA80-21D9-4745-B9DA-57060EA57FF8}"/>
   </bookViews>
   <sheets>
     <sheet name="ItemDatas" sheetId="1" r:id="rId1"/>
@@ -1240,23 +1240,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36525DF8-9879-4440-9A1B-CB7EE677C95C}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.9140625" customWidth="1"/>
+    <col min="2" max="2" width="17.875" customWidth="1"/>
     <col min="3" max="3" width="27.25" customWidth="1"/>
     <col min="4" max="4" width="44.25" customWidth="1"/>
-    <col min="5" max="5" width="6.58203125" customWidth="1"/>
-    <col min="6" max="6" width="35.9140625" customWidth="1"/>
-    <col min="7" max="7" width="19.4140625" customWidth="1"/>
+    <col min="5" max="5" width="6.625" customWidth="1"/>
+    <col min="6" max="6" width="35.875" customWidth="1"/>
+    <col min="7" max="7" width="19.375" customWidth="1"/>
     <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>90</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10202001</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10202002</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10202003</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>10202004</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10202005</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10202006</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10202007</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10202008</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10302000</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10303000</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10304000</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10306000</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>10307000</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>10308000</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10309000</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>10011000</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>10012000</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>10013000</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>10014000</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>10021000</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>10022000</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>5000</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>10161000</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>10113002</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>10113003</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>10113004</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>10113006</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>10113007</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>10113008</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>10113009</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>10114101</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>10114102</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>10114103</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>10114104</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>10114201</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>10114202</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>10116001</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>10000000</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>10001000</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>10002000</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>10010000</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>10100000</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>10110000</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>10110001</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>10110002</v>
       </c>
@@ -2866,7 +2866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>10110003</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>10110004</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>10200000</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>10300000</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>10400000</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>10163000</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>10116003</v>
       </c>
@@ -3128,14 +3128,14 @@
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.58203125" customWidth="1"/>
+    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>101</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10000000</v>
       </c>
@@ -3187,7 +3187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10001000</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10002000</v>
       </c>
@@ -3239,7 +3239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>10010000</v>
       </c>
@@ -3265,7 +3265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10011000</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10012000</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10013000</v>
       </c>
@@ -3343,7 +3343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10014000</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10021000</v>
       </c>
@@ -3395,7 +3395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10022000</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10100000</v>
       </c>
@@ -3447,7 +3447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10161000</v>
       </c>
@@ -3473,7 +3473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>10202005</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>10202006</v>
       </c>
@@ -3525,7 +3525,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10202007</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>10202008</v>
       </c>
@@ -3577,7 +3577,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>10302000</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>10303000</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>10304000</v>
       </c>
@@ -3655,7 +3655,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>10306000</v>
       </c>
@@ -3681,7 +3681,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>10307000</v>
       </c>
@@ -3707,7 +3707,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>10308000</v>
       </c>
@@ -3733,7 +3733,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>10309000</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>10400000</v>
       </c>
@@ -3798,21 +3798,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAB882E2-DC2B-4364-A1E7-50F2FE65D6AC}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.58203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.08203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.4140625" customWidth="1"/>
+    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.375" customWidth="1"/>
     <col min="5" max="5" width="22.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>101</v>
       </c>
@@ -3832,7 +3832,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10110000</v>
       </c>
@@ -3849,10 +3849,10 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10110001</v>
       </c>
@@ -3869,10 +3869,10 @@
         <v>3</v>
       </c>
       <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10110002</v>
       </c>
@@ -3889,10 +3889,10 @@
         <v>3</v>
       </c>
       <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>10110003</v>
       </c>
@@ -3909,10 +3909,10 @@
         <v>2</v>
       </c>
       <c r="F5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10110004</v>
       </c>
@@ -3929,10 +3929,10 @@
         <v>2</v>
       </c>
       <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10114101</v>
       </c>
@@ -3949,10 +3949,10 @@
         <v>2</v>
       </c>
       <c r="F7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10114102</v>
       </c>
@@ -3969,10 +3969,10 @@
         <v>155</v>
       </c>
       <c r="F8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10114103</v>
       </c>
@@ -3989,10 +3989,10 @@
         <v>156</v>
       </c>
       <c r="F9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10114104</v>
       </c>
@@ -4009,10 +4009,10 @@
         <v>155</v>
       </c>
       <c r="F10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10114201</v>
       </c>
@@ -4029,10 +4029,10 @@
         <v>157</v>
       </c>
       <c r="F11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10114202</v>
       </c>
@@ -4049,10 +4049,10 @@
         <v>158</v>
       </c>
       <c r="F12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10113002</v>
       </c>
@@ -4069,10 +4069,10 @@
         <v>2</v>
       </c>
       <c r="F13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>10113003</v>
       </c>
@@ -4089,10 +4089,10 @@
         <v>2</v>
       </c>
       <c r="F14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>10113004</v>
       </c>
@@ -4109,10 +4109,10 @@
         <v>2</v>
       </c>
       <c r="F15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10113006</v>
       </c>
@@ -4129,10 +4129,10 @@
         <v>159</v>
       </c>
       <c r="F16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>10113007</v>
       </c>
@@ -4149,10 +4149,10 @@
         <v>160</v>
       </c>
       <c r="F17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>10113008</v>
       </c>
@@ -4169,10 +4169,10 @@
         <v>161</v>
       </c>
       <c r="F18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>10113009</v>
       </c>
@@ -4189,10 +4189,10 @@
         <v>161</v>
       </c>
       <c r="F19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>10116001</v>
       </c>
@@ -4209,10 +4209,10 @@
         <v>204</v>
       </c>
       <c r="F20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>10116003</v>
       </c>
@@ -4229,7 +4229,7 @@
         <v>204</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix trading UI (#104)
* [FIX]Trading UI And MainScene 기믹 설정 수정

* [FIX] RealPlayer 애니메이션 컨트롤러 공백 제거
</commit_message>
<xml_diff>
--- a/Assets/Resources/ItemData/ItemExcel.xlsx
+++ b/Assets/Resources/ItemData/ItemExcel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Unity\EscapeIsekai\Assets\Resources\ItemData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity\Team\EscapeIsekai\Assets\Resources\ItemData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32380F1A-6EAB-485C-9E9D-35D6F4630B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4C086E-03E5-44C5-BB4D-6CA00611F8CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{23FCFA80-21D9-4745-B9DA-57060EA57FF8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{23FCFA80-21D9-4745-B9DA-57060EA57FF8}"/>
   </bookViews>
   <sheets>
     <sheet name="ItemDatas" sheetId="1" r:id="rId1"/>
@@ -1240,23 +1240,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36525DF8-9879-4440-9A1B-CB7EE677C95C}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.9140625" customWidth="1"/>
+    <col min="2" max="2" width="17.875" customWidth="1"/>
     <col min="3" max="3" width="27.25" customWidth="1"/>
     <col min="4" max="4" width="44.25" customWidth="1"/>
-    <col min="5" max="5" width="6.58203125" customWidth="1"/>
-    <col min="6" max="6" width="35.9140625" customWidth="1"/>
-    <col min="7" max="7" width="19.4140625" customWidth="1"/>
+    <col min="5" max="5" width="6.625" customWidth="1"/>
+    <col min="6" max="6" width="35.875" customWidth="1"/>
+    <col min="7" max="7" width="19.375" customWidth="1"/>
     <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>90</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10202001</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10202002</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10202003</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>10202004</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10202005</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10202006</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10202007</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10202008</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10302000</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10303000</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10304000</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10306000</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>10307000</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>10308000</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10309000</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>10011000</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>10012000</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>10013000</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>10014000</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>10021000</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>10022000</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>5000</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>10161000</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>10113002</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>10113003</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>10113004</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>10113006</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>10113007</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>10113008</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>10113009</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>10114101</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>10114102</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>10114103</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>10114104</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>10114201</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>10114202</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>10116001</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>10000000</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>10001000</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>10002000</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>10010000</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>10100000</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>10110000</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>10110001</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>10110002</v>
       </c>
@@ -2866,7 +2866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>10110003</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>10110004</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>10200000</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>10300000</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>10400000</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>10163000</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>10116003</v>
       </c>
@@ -3128,14 +3128,14 @@
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.58203125" customWidth="1"/>
+    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>101</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10000000</v>
       </c>
@@ -3187,7 +3187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10001000</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10002000</v>
       </c>
@@ -3239,7 +3239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>10010000</v>
       </c>
@@ -3265,7 +3265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10011000</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10012000</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10013000</v>
       </c>
@@ -3343,7 +3343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10014000</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10021000</v>
       </c>
@@ -3395,7 +3395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10022000</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10100000</v>
       </c>
@@ -3447,7 +3447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10161000</v>
       </c>
@@ -3473,7 +3473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>10202005</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>10202006</v>
       </c>
@@ -3525,7 +3525,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10202007</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>10202008</v>
       </c>
@@ -3577,7 +3577,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>10302000</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>10303000</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>10304000</v>
       </c>
@@ -3655,7 +3655,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>10306000</v>
       </c>
@@ -3681,7 +3681,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>10307000</v>
       </c>
@@ -3707,7 +3707,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>10308000</v>
       </c>
@@ -3733,7 +3733,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>10309000</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>10400000</v>
       </c>
@@ -3798,21 +3798,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAB882E2-DC2B-4364-A1E7-50F2FE65D6AC}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.58203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.08203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.4140625" customWidth="1"/>
+    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.375" customWidth="1"/>
     <col min="5" max="5" width="22.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>101</v>
       </c>
@@ -3832,7 +3832,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10110000</v>
       </c>
@@ -3849,10 +3849,10 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10110001</v>
       </c>
@@ -3869,10 +3869,10 @@
         <v>3</v>
       </c>
       <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10110002</v>
       </c>
@@ -3889,10 +3889,10 @@
         <v>3</v>
       </c>
       <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>10110003</v>
       </c>
@@ -3909,10 +3909,10 @@
         <v>2</v>
       </c>
       <c r="F5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10110004</v>
       </c>
@@ -3929,10 +3929,10 @@
         <v>2</v>
       </c>
       <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10114101</v>
       </c>
@@ -3949,10 +3949,10 @@
         <v>2</v>
       </c>
       <c r="F7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10114102</v>
       </c>
@@ -3969,10 +3969,10 @@
         <v>155</v>
       </c>
       <c r="F8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10114103</v>
       </c>
@@ -3989,10 +3989,10 @@
         <v>156</v>
       </c>
       <c r="F9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10114104</v>
       </c>
@@ -4009,10 +4009,10 @@
         <v>155</v>
       </c>
       <c r="F10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10114201</v>
       </c>
@@ -4029,10 +4029,10 @@
         <v>157</v>
       </c>
       <c r="F11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10114202</v>
       </c>
@@ -4049,10 +4049,10 @@
         <v>158</v>
       </c>
       <c r="F12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10113002</v>
       </c>
@@ -4069,10 +4069,10 @@
         <v>2</v>
       </c>
       <c r="F13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>10113003</v>
       </c>
@@ -4089,10 +4089,10 @@
         <v>2</v>
       </c>
       <c r="F14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>10113004</v>
       </c>
@@ -4109,10 +4109,10 @@
         <v>2</v>
       </c>
       <c r="F15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10113006</v>
       </c>
@@ -4129,10 +4129,10 @@
         <v>159</v>
       </c>
       <c r="F16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>10113007</v>
       </c>
@@ -4149,10 +4149,10 @@
         <v>160</v>
       </c>
       <c r="F17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>10113008</v>
       </c>
@@ -4169,10 +4169,10 @@
         <v>161</v>
       </c>
       <c r="F18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>10113009</v>
       </c>
@@ -4189,10 +4189,10 @@
         <v>161</v>
       </c>
       <c r="F19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>10116001</v>
       </c>
@@ -4209,10 +4209,10 @@
         <v>204</v>
       </c>
       <c r="F20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>10116003</v>
       </c>
@@ -4229,7 +4229,7 @@
         <v>204</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>